<commit_message>
fundament for calculating dipole matrix elements
</commit_message>
<xml_diff>
--- a/transistions.xlsx
+++ b/transistions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="314">
   <si>
     <t>0.035</t>
   </si>
@@ -952,13 +952,31 @@
   </si>
   <si>
     <t>O. S. Heavanes</t>
+  </si>
+  <si>
+    <r>
+      <t>6p 2 P ⴰ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3/2</t>
+    </r>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1005,6 +1023,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1102,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1189,9 +1214,6 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1227,6 +1249,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1535,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="I174" sqref="I174"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="I197" sqref="I197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4886,10 +4913,10 @@
       <c r="F151" s="4"/>
       <c r="G151" s="4"/>
       <c r="H151" s="6"/>
-      <c r="I151" s="47" t="s">
+      <c r="I151" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="J151" s="47"/>
+      <c r="J151" s="46"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
@@ -4906,10 +4933,10 @@
       <c r="F152" s="4"/>
       <c r="G152" s="4"/>
       <c r="H152" s="6"/>
-      <c r="I152" s="47" t="s">
+      <c r="I152" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="J152" s="47"/>
+      <c r="J152" s="46"/>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="21">
@@ -5338,7 +5365,7 @@
       <c r="J170" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="K170" s="44">
+      <c r="K170" s="43">
         <v>940000</v>
       </c>
     </row>
@@ -5457,7 +5484,7 @@
       <c r="J175" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="K175" s="45">
+      <c r="K175" s="44">
         <v>2970000</v>
       </c>
     </row>
@@ -6848,7 +6875,7 @@
       <c r="E234" s="14"/>
       <c r="F234" s="14"/>
       <c r="G234" s="14"/>
-      <c r="H234" s="35">
+      <c r="H234" s="34">
         <v>2040000</v>
       </c>
       <c r="I234" s="14" t="s">
@@ -6929,7 +6956,7 @@
       <c r="E237" s="16"/>
       <c r="F237" s="16"/>
       <c r="G237" s="16"/>
-      <c r="H237" s="35">
+      <c r="H237" s="34">
         <v>3600000</v>
       </c>
       <c r="I237" s="16" t="s">
@@ -7043,7 +7070,7 @@
       <c r="E242" s="14"/>
       <c r="F242" s="14"/>
       <c r="G242" s="14"/>
-      <c r="H242" s="35">
+      <c r="H242" s="34">
         <v>12700000</v>
       </c>
       <c r="I242" s="14" t="s">
@@ -7089,16 +7116,16 @@
       <c r="C244" s="17">
         <v>11209.572</v>
       </c>
-      <c r="D244" s="41" t="s">
+      <c r="D244" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="E244" s="42">
+      <c r="E244" s="41">
         <v>0.63500000000000001</v>
       </c>
-      <c r="F244" s="42">
+      <c r="F244" s="41">
         <v>1.5</v>
       </c>
-      <c r="G244" s="42">
+      <c r="G244" s="41">
         <v>0.5</v>
       </c>
       <c r="H244" s="30">
@@ -7124,13 +7151,13 @@
       <c r="D245" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="E245" s="46">
+      <c r="E245" s="45">
         <v>0.80700000000000005</v>
       </c>
-      <c r="F245" s="46">
+      <c r="F245" s="45">
         <v>2.5</v>
       </c>
-      <c r="G245" s="46">
+      <c r="G245" s="45">
         <v>1.5</v>
       </c>
       <c r="H245" s="30">
@@ -7203,7 +7230,7 @@
       <c r="E248" s="16"/>
       <c r="F248" s="16"/>
       <c r="G248" s="16"/>
-      <c r="H248" s="35">
+      <c r="H248" s="34">
         <v>2660000</v>
       </c>
       <c r="I248" s="16" t="s">
@@ -7789,7 +7816,7 @@
       <c r="G271" s="18">
         <v>1.5</v>
       </c>
-      <c r="H271" s="35">
+      <c r="H271" s="34">
         <v>130000</v>
       </c>
       <c r="I271" s="18" t="s">
@@ -7823,7 +7850,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="2">
         <v>13575.189</v>
       </c>
@@ -7847,7 +7874,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="13">
         <v>13592.008</v>
       </c>
@@ -7878,34 +7905,36 @@
       <c r="J274" s="14" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A275" s="36">
+      <c r="K274" s="47"/>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A275" s="35">
         <v>13606.276</v>
       </c>
-      <c r="B275" s="36" t="s">
+      <c r="B275" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="C275" s="36">
+      <c r="C275" s="35">
         <v>7349.5496999999996</v>
       </c>
-      <c r="D275" s="36" t="s">
+      <c r="D275" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="E275" s="37"/>
-      <c r="F275" s="37"/>
-      <c r="G275" s="37"/>
-      <c r="H275" s="38">
+      <c r="E275" s="36"/>
+      <c r="F275" s="36"/>
+      <c r="G275" s="36"/>
+      <c r="H275" s="37">
         <v>1100000</v>
       </c>
-      <c r="I275" s="37" t="s">
+      <c r="I275" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="J275" s="37" t="s">
+      <c r="J275" s="36" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K275" s="47"/>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="17">
         <v>13762.57</v>
       </c>
@@ -7927,7 +7956,7 @@
       <c r="G276" s="18">
         <v>0.5</v>
       </c>
-      <c r="H276" s="35">
+      <c r="H276" s="34">
         <v>1590000</v>
       </c>
       <c r="I276" s="18" t="s">
@@ -7936,8 +7965,9 @@
       <c r="J276" s="18" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K276" s="47"/>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="7">
         <v>13781.739</v>
       </c>
@@ -7950,13 +7980,13 @@
       <c r="D277" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="E277" s="43">
+      <c r="E277" s="42">
         <v>1.62035</v>
       </c>
-      <c r="F277" s="43">
+      <c r="F277" s="42">
         <v>0.5</v>
       </c>
-      <c r="G277" s="43">
+      <c r="G277" s="42">
         <v>1.5</v>
       </c>
       <c r="H277" s="30">
@@ -7968,8 +7998,9 @@
       <c r="J277" s="8" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K277" s="47"/>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="11">
         <v>13917.2397</v>
       </c>
@@ -7992,8 +8023,9 @@
       <c r="J278" s="12" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K278" s="47"/>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="7">
         <v>13940.5767</v>
       </c>
@@ -8025,8 +8057,11 @@
       <c r="J279" s="8" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K279" s="49" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="2">
         <v>14104.531999999999</v>
       </c>
@@ -8049,8 +8084,9 @@
       <c r="J280" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K280" s="47"/>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="2">
         <v>14157.616</v>
       </c>
@@ -8073,8 +8109,9 @@
       <c r="J281" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K281" s="47"/>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="2">
         <v>14190.434999999999</v>
       </c>
@@ -8097,8 +8134,9 @@
       <c r="J282" s="3" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K282" s="47"/>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="11">
         <v>14515.050999999999</v>
       </c>
@@ -8121,8 +8159,9 @@
       <c r="J283" s="12" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K283" s="47"/>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="11">
         <v>14530.052</v>
       </c>
@@ -8145,8 +8184,9 @@
       <c r="J284" s="12" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K284" s="47"/>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
         <v>14674.373</v>
       </c>
@@ -8169,40 +8209,42 @@
       <c r="J285" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A286" s="13">
+      <c r="K285" s="47"/>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A286" s="15">
         <v>14698.924999999999</v>
       </c>
-      <c r="B286" s="13" t="s">
+      <c r="B286" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C286" s="13">
+      <c r="C286" s="15">
         <v>6803.2186000000002</v>
       </c>
-      <c r="D286" s="13" t="s">
+      <c r="D286" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="E286" s="34">
+      <c r="E286" s="48">
         <v>4.2409999999999997</v>
       </c>
-      <c r="F286" s="34">
+      <c r="F286" s="48">
         <v>0.5</v>
       </c>
-      <c r="G286" s="34">
+      <c r="G286" s="48">
         <v>0.5</v>
       </c>
-      <c r="H286" s="35">
-        <v>6230000</v>
-      </c>
-      <c r="I286" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="J286" s="14" t="s">
+      <c r="H286" s="34">
+        <v>11400000</v>
+      </c>
+      <c r="I286" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="J286" s="16" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K286" s="47"/>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
         <v>14729.413</v>
       </c>
@@ -8226,7 +8268,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
         <v>15245.859</v>
       </c>
@@ -9354,16 +9396,16 @@
       <c r="D334" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="E334" s="39">
+      <c r="E334" s="38">
         <v>14.32</v>
       </c>
-      <c r="F334" s="39">
+      <c r="F334" s="38">
         <v>0.5</v>
       </c>
-      <c r="G334" s="39">
+      <c r="G334" s="38">
         <v>1.5</v>
       </c>
-      <c r="H334" s="35">
+      <c r="H334" s="34">
         <v>4050000</v>
       </c>
       <c r="I334" s="8" t="s">
@@ -9464,16 +9506,16 @@
       <c r="D338" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="E338" s="39">
+      <c r="E338" s="38">
         <v>10.314</v>
       </c>
-      <c r="F338" s="39">
+      <c r="F338" s="38">
         <v>0.5</v>
       </c>
-      <c r="G338" s="39">
+      <c r="G338" s="38">
         <v>0.5</v>
       </c>
-      <c r="H338" s="35">
+      <c r="H338" s="34">
         <v>3520000</v>
       </c>
       <c r="I338" s="8" t="s">
@@ -9704,7 +9746,7 @@
       <c r="E347" s="4"/>
       <c r="F347" s="4"/>
       <c r="G347" s="4"/>
-      <c r="H347" s="40">
+      <c r="H347" s="39">
         <v>1380000</v>
       </c>
       <c r="I347" s="4" t="s">

</xml_diff>